<commit_message>
exel file changed secondly
</commit_message>
<xml_diff>
--- a/siraj addnew-library.xlsx
+++ b/siraj addnew-library.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\my workshop\lib\othersoft\projectwork\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5B2223-78F1-4A4A-B75D-68C5A6BCCD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2724" yWindow="240" windowWidth="21396" windowHeight="10416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="21855" windowHeight="10965"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,17 +55,23 @@
     <t>Library Section</t>
   </si>
   <si>
-    <t>da sheriyaayi</t>
+    <t>ok aanu seen illa</t>
   </si>
   <si>
-    <t xml:space="preserve">ammal ok da  </t>
+    <t>da sheriyaayi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,8 +116,152 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,18 +270,204 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79995117038483843"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="8" tint="0.799951170384838"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.0999786370433668"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -357,12 +687,263 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -378,34 +959,69 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -663,130 +1279,132 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="C2:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" customWidth="1"/>
-    <col min="7" max="7" width="28.33203125" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.3333333333333" customWidth="1"/>
+    <col min="7" max="7" width="28.3333333333333" customWidth="1"/>
+    <col min="8" max="8" width="21.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:10">
-      <c r="D2" s="21" t="s">
+    <row r="2" spans="4:6">
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="3:10">
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+    <row r="3" spans="4:6">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="3:10">
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+    <row r="4" spans="4:6">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="3:10" ht="31.2">
-      <c r="J5" s="12"/>
+    <row r="5" ht="31.5" spans="10:10">
+      <c r="J5" s="15"/>
     </row>
-    <row r="6" spans="3:10" ht="21">
-      <c r="J6" s="13"/>
+    <row r="6" ht="21.75" spans="10:10">
+      <c r="J6" s="16"/>
     </row>
-    <row r="7" spans="3:10" ht="31.2">
-      <c r="C7" s="18" t="s">
+    <row r="7" ht="33" spans="3:10">
+      <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="14"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18"/>
     </row>
-    <row r="8" spans="3:10" ht="21">
-      <c r="C8" s="1" t="s">
+    <row r="8" ht="22.5" spans="3:10">
+      <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="14"/>
+      <c r="J8" s="18"/>
     </row>
-    <row r="9" spans="3:10" ht="18">
-      <c r="C9" s="4" t="s">
+    <row r="9" ht="20.25" spans="3:10">
+      <c r="C9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="5">
+      <c r="G9" s="10"/>
+      <c r="H9" s="8">
         <v>2</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="14"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="18"/>
     </row>
-    <row r="10" spans="3:10" ht="18">
-      <c r="C10" s="8" t="s">
+    <row r="10" ht="20.25" spans="3:10">
+      <c r="C10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="9">
+      <c r="G10" s="14"/>
+      <c r="H10" s="12">
         <v>3</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="14"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="18"/>
     </row>
+    <row r="11" ht="15.75"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C7:I7"/>
     <mergeCell ref="D2:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
work1 submitted word and exel files
</commit_message>
<xml_diff>
--- a/siraj addnew-library.xlsx
+++ b/siraj addnew-library.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Siraj</t>
   </si>
@@ -49,16 +49,22 @@
     <t>2)    Author</t>
   </si>
   <si>
+    <t>AUTHOR</t>
+  </si>
+  <si>
     <t>1.5 hr</t>
   </si>
   <si>
+    <t>10 mnt</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
     <t>Library Section</t>
   </si>
   <si>
-    <t>ok aanu seen illa</t>
-  </si>
-  <si>
-    <t>da sheriyaayi</t>
+    <t>SectionMaster</t>
   </si>
 </sst>
 </file>
@@ -117,6 +123,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -125,22 +152,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -148,24 +166,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -187,10 +190,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -202,60 +236,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -282,187 +288,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -684,6 +690,69 @@
       </top>
       <bottom style="thick">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -712,60 +781,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -776,19 +791,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -806,130 +812,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1288,7 +1294,7 @@
   <dimension ref="C2:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1299,6 +1305,7 @@
     <col min="6" max="6" width="22.3333333333333" customWidth="1"/>
     <col min="7" max="7" width="28.3333333333333" customWidth="1"/>
     <col min="8" max="8" width="21.6666666666667" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:6">
@@ -1367,35 +1374,43 @@
       <c r="D9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="F9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="10"/>
+        <v>12</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="H9" s="8">
         <v>2</v>
       </c>
-      <c r="I9" s="20"/>
+      <c r="I9" s="20" t="s">
+        <v>14</v>
+      </c>
       <c r="J9" s="18"/>
     </row>
     <row r="10" ht="20.25" spans="3:10">
       <c r="C10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="G10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="14"/>
       <c r="H10" s="12">
         <v>3</v>
       </c>
-      <c r="I10" s="21"/>
+      <c r="I10" s="21" t="s">
+        <v>14</v>
+      </c>
       <c r="J10" s="18"/>
     </row>
     <row r="11" ht="15.75"/>

</xml_diff>